<commit_message>
Transform project to maven and add import xlsx option
</commit_message>
<xml_diff>
--- a/dbFiles/test.xlsx
+++ b/dbFiles/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\java\physicsCalculator\dbFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F929519A-B6D6-44A5-AB8C-0FE3C5164AA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EE7E3E-7120-438E-B175-595FD88AC84E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Hello world</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,26 +345,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>213</v>
       </c>
       <c r="C1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>123.213122</v>
+      </c>
+      <c r="D1">
+        <v>52</v>
+      </c>
+      <c r="E1">
+        <v>231</v>
+      </c>
+      <c r="F1">
+        <v>231</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -367,7 +385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -375,6 +393,32 @@
         <v>4</v>
       </c>
       <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C7">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Misc.significantNumbers method and excel data import
</commit_message>
<xml_diff>
--- a/dbFiles/test.xlsx
+++ b/dbFiles/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\java\physicsCalculator\dbFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EE7E3E-7120-438E-B175-595FD88AC84E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F3258-AE54-4824-A31D-12AB23D9246A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="6216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,9 +345,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -359,7 +361,7 @@
         <v>213</v>
       </c>
       <c r="C1">
-        <v>123.213122</v>
+        <v>123.21312</v>
       </c>
       <c r="D1">
         <v>52</v>
@@ -384,6 +386,15 @@
       <c r="C2">
         <v>4</v>
       </c>
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
+      </c>
+      <c r="F2">
+        <v>123</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -415,11 +426,6 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>